<commit_message>
intro scene title button
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>SceneName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -51,6 +51,14 @@
   </si>
   <si>
     <t>IntroScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>○</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AtHomeScene</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -411,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -447,6 +455,17 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
cafe scene bug fix
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>SceneName</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,6 +79,14 @@
   </si>
   <si>
     <t>ParkScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CafeScene</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ConvenienceScene</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -149,7 +157,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -157,6 +165,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -439,7 +450,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -530,6 +541,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>